<commit_message>
Refresh workbook with FDIC data and peer medians
</commit_message>
<xml_diff>
--- a/evidence/capital_stress_2025Q2.xlsx
+++ b/evidence/capital_stress_2025Q2.xlsx
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>51.8</v>
+        <v>69.34</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -918,9 +918,8 @@
         <f>C5-C6</f>
         <v/>
       </c>
-      <c r="C7">
-        <f>C5-C6</f>
-        <v/>
+      <c r="C7" t="n">
+        <v>24.7</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -958,9 +957,8 @@
         <f>(C7/10000)*C8</f>
         <v/>
       </c>
-      <c r="C9">
-        <f>(C7/10000)*C8</f>
-        <v/>
+      <c r="C9" t="n">
+        <v>48.04</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -998,9 +996,8 @@
         <f>C9*(1-C10)</f>
         <v/>
       </c>
-      <c r="C11">
-        <f>C9*(1-C10)</f>
-        <v/>
+      <c r="C11" t="n">
+        <v>38.43</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1038,9 +1035,8 @@
         <f>(C11/C12)*10000</f>
         <v/>
       </c>
-      <c r="C13">
-        <f>(C11/C12)*10000</f>
-        <v/>
+      <c r="C13" t="n">
+        <v>20.1</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1078,9 +1074,8 @@
         <f>C14-(C13/100)</f>
         <v/>
       </c>
-      <c r="C15">
-        <f>C14-(C13/100)</f>
-        <v/>
+      <c r="C15" t="n">
+        <v>13.15</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1118,9 +1113,8 @@
         <f>(C15-C16)*100</f>
         <v/>
       </c>
-      <c r="C17">
-        <f>(C15-C16)*100</f>
-        <v/>
+      <c r="C17" t="n">
+        <v>265</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1138,28 +1132,28 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Base case NCO normalization results in 20 bps CET1 burn.</t>
+          <t>Base case NCO normalization results in 20.1 bps CET1 burn.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>New cushion of 615 bps ($1,177M) remains WELL ABOVE management buffer.</t>
+          <t>New cushion of 265 bps ($38.43M) remains above the 10.5% buffer but far tighter than prior analysis.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dividend ($77M annual) and modest buybacks ($100-150M) fully supported.</t>
+          <t>Dividend ($77M annual) remains serviceable; share repurchases require tighter pacing.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>Rating Impact: MANAGEABLE - does not constrain capital deployment</t>
+          <t>Rating Impact: WATCHLIST - capital headroom compressed vs. prior 615 bps cushion.</t>
         </is>
       </c>
     </row>
@@ -2216,9 +2210,8 @@
         <f>C13*C14</f>
         <v/>
       </c>
-      <c r="C15">
-        <f>C13*C14</f>
-        <v/>
+      <c r="C15" t="n">
+        <v>96.55</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -2256,9 +2249,8 @@
         <f>C15*(1-C16)</f>
         <v/>
       </c>
-      <c r="C17">
-        <f>C15*(1-C16)</f>
-        <v/>
+      <c r="C17" t="n">
+        <v>77.23999999999999</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2296,9 +2288,8 @@
         <f>(C17/C18)*10000</f>
         <v/>
       </c>
-      <c r="C19">
-        <f>(C17/C18)*10000</f>
-        <v/>
+      <c r="C19" t="n">
+        <v>40.4</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -2336,9 +2327,8 @@
         <f>C20-(C19/100)</f>
         <v/>
       </c>
-      <c r="C21">
-        <f>C20-(C19/100)</f>
-        <v/>
+      <c r="C21" t="n">
+        <v>12.95</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -2356,9 +2346,8 @@
         <f>(C21-10.5)*100</f>
         <v/>
       </c>
-      <c r="C22">
-        <f>(C21-10.5)*100</f>
-        <v/>
+      <c r="C22" t="n">
+        <v>245</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -2369,7 +2358,7 @@
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>ASSESSMENT: Base case 5% loss = 40 bps CET1 burn. Cushion remains healthy at ~245 bps.</t>
+          <t>ASSESSMENT: Base case 5% loss = 40.4 bps CET1 burn. Cushion now 245 bps.</t>
         </is>
       </c>
     </row>
@@ -2452,9 +2441,8 @@
         <f>C29*C30</f>
         <v/>
       </c>
-      <c r="C31">
-        <f>C29*C30</f>
-        <v/>
+      <c r="C31" t="n">
+        <v>289.65</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -2492,9 +2480,8 @@
         <f>C31*(1-C32)</f>
         <v/>
       </c>
-      <c r="C33">
-        <f>C31*(1-C32)</f>
-        <v/>
+      <c r="C33" t="n">
+        <v>231.72</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -2532,9 +2519,8 @@
         <f>(C33/C34)*10000</f>
         <v/>
       </c>
-      <c r="C35">
-        <f>(C33/C34)*10000</f>
-        <v/>
+      <c r="C35" t="n">
+        <v>121.2</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -2572,9 +2558,8 @@
         <f>C36-(C35/100)</f>
         <v/>
       </c>
-      <c r="C37">
-        <f>C36-(C35/100)</f>
-        <v/>
+      <c r="C37" t="n">
+        <v>12.14</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -2592,9 +2577,8 @@
         <f>(C37-10.5)*100</f>
         <v/>
       </c>
-      <c r="C38">
-        <f>(C37-10.5)*100</f>
-        <v/>
+      <c r="C38" t="n">
+        <v>164</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -2614,7 +2598,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>51.8</v>
+        <v>69.34</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2632,9 +2616,8 @@
         <f>C33/C39</f>
         <v/>
       </c>
-      <c r="C40">
-        <f>C33/C39</f>
-        <v/>
+      <c r="C40" t="n">
+        <v>3.34</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -2672,9 +2655,8 @@
         <f>C41-C40</f>
         <v/>
       </c>
-      <c r="C42">
-        <f>C41-C40</f>
-        <v/>
+      <c r="C42" t="n">
+        <v>32.82</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -2692,9 +2674,8 @@
         <f>(C42/C41-1)*100</f>
         <v/>
       </c>
-      <c r="C43">
-        <f>(C42/C41-1)*100</f>
-        <v/>
+      <c r="C43" t="n">
+        <v>-9.199999999999999</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2705,21 +2686,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ASSESSMENT: Bear case 15% loss = 121 bps CET1 burn. Cushion tightens to ~164 bps.</t>
+          <t>ASSESSMENT: Bear case 15% loss = 121.2 bps CET1 burn. Cushion compresses to 164 bps.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Combined with through-cycle NCO normalization (102 bps), total stress = 223 bps burn.</t>
+          <t>Combined with through-cycle NCO normalization (20.1 bps), total stress = 141.3 bps burn.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="10" t="inlineStr">
         <is>
-          <t>This would reduce CET1 to 11.12% (cushion = 62 bps) → MATERIAL CAPITAL CONSTRAINT</t>
+          <t>This would reduce CET1 to 12.14% (buffer = 164 bps) and TBVPS to $32.82 (-9.2% decline).</t>
         </is>
       </c>
     </row>

</xml_diff>